<commit_message>
Cang| Add power point file
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -232,9 +232,6 @@
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -244,14 +241,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -559,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -569,49 +569,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="P1" s="6"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="P1" s="5"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2" t="s">
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="10" t="s">
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="10"/>
-      <c r="P2" s="5"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="4"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -620,479 +620,478 @@
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="11" t="s">
+      <c r="N3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="O3" s="9" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="12"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="10"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="12"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="10"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="12"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="10"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="12"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="10"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="12"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="10"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="12"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="10"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="12"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="10"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="12"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="10"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="12"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="10"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="12"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="10"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="12"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="10"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="12"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="10"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="12"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="10"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="12"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="10"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="12"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="10"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="12"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="10"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="13"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="11"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="12"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="10"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="12"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="10"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="12"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="10"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="12"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="10"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="12"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="10"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="12"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="10"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="15"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
update planing and power point
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Tuần 2</t>
   </si>
@@ -116,13 +116,22 @@
   </si>
   <si>
     <t>Chẩn đoán một loại bệnh về phổi trong y khoa thông qua hình ảnh (X-ray)</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>Research CNN</t>
+  </si>
+  <si>
+    <t>Apply CNN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,8 +154,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,6 +172,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -225,9 +246,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -243,7 +265,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -252,9 +273,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -557,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P27"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -569,48 +592,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
       <c r="P1" s="5"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14" t="s">
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="15" t="s">
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="15"/>
+      <c r="O2" s="14"/>
       <c r="P2" s="4"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -684,12 +707,12 @@
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
@@ -778,13 +801,13 @@
         <v>20</v>
       </c>
       <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -860,16 +883,18 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
       <c r="N14" s="3"/>
       <c r="O14" s="10"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -877,16 +902,15 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
       <c r="N15" s="3"/>
       <c r="O15" s="10"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
+      <c r="A16" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -894,17 +918,16 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
       <c r="N16" s="3"/>
       <c r="O16" s="10"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -914,15 +937,16 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
       <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
       <c r="O17" s="10"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
+      <c r="A18" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -933,13 +957,15 @@
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
       <c r="O18" s="10"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -950,15 +976,10 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="10"/>
+      <c r="O19" s="15"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="A20" s="1"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -972,10 +993,8 @@
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
-      <c r="O20" s="11"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -989,10 +1008,9 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
-      <c r="O21" s="10"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
+      <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -1078,20 +1096,37 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="12"/>
-      <c r="O27" s="13"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="10"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>